<commit_message>
Added all API routes. Inputted all objects into database. Wrote script for storing a json class descriptor in the database.
</commit_message>
<xml_diff>
--- a/documentation/Gantt Chart.xlsx
+++ b/documentation/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{5407DB28-46D2-4894-ACBD-CE904A346A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578358BC-F156-4AB3-A780-858E035EED23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>Implement SCG functionality</t>
   </si>
   <si>
-    <t>Add user accounts</t>
-  </si>
-  <si>
     <t>Project Initialisation</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Users can save custom game objects in the database</t>
+  </si>
+  <si>
+    <t>Add user accounts (stretch goal)</t>
   </si>
 </sst>
 </file>
@@ -748,45 +748,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -798,134 +759,173 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="11" borderId="2" xfId="3" applyFill="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="12" borderId="2" xfId="3" applyFill="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="6" borderId="7" xfId="13" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="11" borderId="2" xfId="3" applyFill="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="12" borderId="2" xfId="3" applyFill="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="7" xfId="13" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1338,8 +1338,8 @@
   </sheetPr>
   <dimension ref="B1:BP38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AG13" sqref="AG13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1355,7 +1355,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:68" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8"/>
@@ -1365,62 +1365,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65">
+      <c r="H2" s="35"/>
+      <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="18"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="69"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="18"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="69"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="20"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="71"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="21" t="s">
+      <c r="AB2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="23"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="74"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="14" t="s">
+      <c r="AJ2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
+      <c r="AK2" s="66"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
     </row>
     <row r="3" spans="2:68" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1451,90 +1451,90 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="39">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="58">
         <v>44120</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40">
+      <c r="J5" s="59"/>
+      <c r="K5" s="59">
         <v>44127</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="41">
+      <c r="L5" s="60"/>
+      <c r="M5" s="54">
         <v>44134</v>
       </c>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41">
+      <c r="N5" s="54"/>
+      <c r="O5" s="54">
         <v>44141</v>
       </c>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41">
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54">
         <v>44148</v>
       </c>
-      <c r="R5" s="41"/>
-      <c r="S5" s="42">
+      <c r="R5" s="54"/>
+      <c r="S5" s="55">
         <v>44155</v>
       </c>
-      <c r="T5" s="42"/>
-      <c r="U5" s="41">
+      <c r="T5" s="55"/>
+      <c r="U5" s="54">
         <v>44162</v>
       </c>
-      <c r="V5" s="58"/>
-      <c r="W5" s="43">
+      <c r="V5" s="56"/>
+      <c r="W5" s="51">
         <v>44169</v>
       </c>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="44">
+      <c r="X5" s="51"/>
+      <c r="Y5" s="50">
         <v>44176</v>
       </c>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="43">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="51">
         <v>44183</v>
       </c>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="44">
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="50">
         <v>44190</v>
       </c>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46">
+      <c r="AD5" s="52"/>
+      <c r="AE5" s="53">
         <v>44197</v>
       </c>
       <c r="AF5" s="47"/>
@@ -1554,255 +1554,255 @@
         <v>44225</v>
       </c>
       <c r="AN5" s="47"/>
-      <c r="AO5" s="60">
+      <c r="AO5" s="49">
         <v>44232</v>
       </c>
-      <c r="AP5" s="49"/>
-      <c r="AQ5" s="50">
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="44">
         <v>44239</v>
       </c>
-      <c r="AR5" s="50"/>
-      <c r="AS5" s="49">
+      <c r="AR5" s="44"/>
+      <c r="AS5" s="43">
         <v>44246</v>
       </c>
-      <c r="AT5" s="49"/>
-      <c r="AU5" s="50">
+      <c r="AT5" s="43"/>
+      <c r="AU5" s="44">
         <v>44253</v>
       </c>
-      <c r="AV5" s="50"/>
-      <c r="AW5" s="61">
+      <c r="AV5" s="44"/>
+      <c r="AW5" s="45">
         <v>44260</v>
       </c>
-      <c r="AX5" s="51"/>
-      <c r="AY5" s="52">
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="39">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="52"/>
-      <c r="BA5" s="51">
+      <c r="AZ5" s="39"/>
+      <c r="BA5" s="46">
         <v>44274</v>
       </c>
-      <c r="BB5" s="51"/>
-      <c r="BC5" s="52">
+      <c r="BB5" s="46"/>
+      <c r="BC5" s="39">
         <v>44281</v>
       </c>
-      <c r="BD5" s="53"/>
-      <c r="BE5" s="54">
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="41">
         <v>44288</v>
       </c>
-      <c r="BF5" s="55"/>
-      <c r="BG5" s="56">
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="42">
         <v>44295</v>
       </c>
-      <c r="BH5" s="56"/>
-      <c r="BI5" s="55">
+      <c r="BH5" s="42"/>
+      <c r="BI5" s="31">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="55"/>
-      <c r="BK5" s="56">
+      <c r="BJ5" s="31"/>
+      <c r="BK5" s="42">
         <v>44309</v>
       </c>
-      <c r="BL5" s="56"/>
-      <c r="BM5" s="55">
+      <c r="BL5" s="42"/>
+      <c r="BM5" s="31">
         <v>44316</v>
       </c>
-      <c r="BN5" s="57"/>
-      <c r="BO5" s="29"/>
+      <c r="BN5" s="32"/>
+      <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="35">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="21">
         <v>1</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="21">
         <v>2</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="21">
         <v>3</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="21">
         <v>4</v>
       </c>
-      <c r="M6" s="36">
+      <c r="M6" s="22">
         <v>5</v>
       </c>
-      <c r="N6" s="36">
+      <c r="N6" s="22">
         <v>6</v>
       </c>
-      <c r="O6" s="36">
+      <c r="O6" s="22">
         <v>7</v>
       </c>
-      <c r="P6" s="36">
+      <c r="P6" s="22">
         <v>8</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="21">
         <v>9</v>
       </c>
-      <c r="R6" s="35">
+      <c r="R6" s="21">
         <v>10</v>
       </c>
-      <c r="S6" s="35">
+      <c r="S6" s="21">
         <v>11</v>
       </c>
-      <c r="T6" s="35">
+      <c r="T6" s="21">
         <v>12</v>
       </c>
-      <c r="U6" s="36">
+      <c r="U6" s="22">
         <v>13</v>
       </c>
-      <c r="V6" s="36">
+      <c r="V6" s="22">
         <v>14</v>
       </c>
-      <c r="W6" s="36">
+      <c r="W6" s="22">
         <v>15</v>
       </c>
-      <c r="X6" s="36">
+      <c r="X6" s="22">
         <v>16</v>
       </c>
-      <c r="Y6" s="35">
+      <c r="Y6" s="21">
         <v>17</v>
       </c>
-      <c r="Z6" s="35">
+      <c r="Z6" s="21">
         <v>18</v>
       </c>
-      <c r="AA6" s="35">
+      <c r="AA6" s="21">
         <v>19</v>
       </c>
-      <c r="AB6" s="35">
+      <c r="AB6" s="21">
         <v>20</v>
       </c>
-      <c r="AC6" s="36">
+      <c r="AC6" s="22">
         <v>21</v>
       </c>
-      <c r="AD6" s="36">
+      <c r="AD6" s="22">
         <v>22</v>
       </c>
-      <c r="AE6" s="36">
+      <c r="AE6" s="22">
         <v>23</v>
       </c>
-      <c r="AF6" s="36">
+      <c r="AF6" s="22">
         <v>24</v>
       </c>
-      <c r="AG6" s="35">
+      <c r="AG6" s="21">
         <v>25</v>
       </c>
-      <c r="AH6" s="35">
+      <c r="AH6" s="21">
         <v>26</v>
       </c>
-      <c r="AI6" s="35">
+      <c r="AI6" s="21">
         <v>27</v>
       </c>
-      <c r="AJ6" s="35">
+      <c r="AJ6" s="21">
         <v>28</v>
       </c>
-      <c r="AK6" s="36">
+      <c r="AK6" s="22">
         <v>29</v>
       </c>
-      <c r="AL6" s="36">
+      <c r="AL6" s="22">
         <v>30</v>
       </c>
-      <c r="AM6" s="36">
+      <c r="AM6" s="22">
         <v>31</v>
       </c>
-      <c r="AN6" s="36">
+      <c r="AN6" s="22">
         <v>32</v>
       </c>
-      <c r="AO6" s="35">
+      <c r="AO6" s="21">
         <v>33</v>
       </c>
-      <c r="AP6" s="35">
+      <c r="AP6" s="21">
         <v>34</v>
       </c>
-      <c r="AQ6" s="35">
+      <c r="AQ6" s="21">
         <v>35</v>
       </c>
-      <c r="AR6" s="35">
+      <c r="AR6" s="21">
         <v>36</v>
       </c>
-      <c r="AS6" s="36">
+      <c r="AS6" s="22">
         <v>37</v>
       </c>
-      <c r="AT6" s="36">
+      <c r="AT6" s="22">
         <v>38</v>
       </c>
-      <c r="AU6" s="36">
+      <c r="AU6" s="22">
         <v>39</v>
       </c>
-      <c r="AV6" s="36">
+      <c r="AV6" s="22">
         <v>40</v>
       </c>
-      <c r="AW6" s="35">
+      <c r="AW6" s="21">
         <v>41</v>
       </c>
-      <c r="AX6" s="35">
+      <c r="AX6" s="21">
         <v>42</v>
       </c>
-      <c r="AY6" s="35">
+      <c r="AY6" s="21">
         <v>43</v>
       </c>
-      <c r="AZ6" s="35">
+      <c r="AZ6" s="21">
         <v>44</v>
       </c>
-      <c r="BA6" s="36">
+      <c r="BA6" s="22">
         <v>45</v>
       </c>
-      <c r="BB6" s="36">
+      <c r="BB6" s="22">
         <v>46</v>
       </c>
-      <c r="BC6" s="36">
+      <c r="BC6" s="22">
         <v>47</v>
       </c>
-      <c r="BD6" s="36">
+      <c r="BD6" s="22">
         <v>48</v>
       </c>
-      <c r="BE6" s="35">
+      <c r="BE6" s="21">
         <v>49</v>
       </c>
-      <c r="BF6" s="35">
+      <c r="BF6" s="21">
         <v>50</v>
       </c>
-      <c r="BG6" s="35">
+      <c r="BG6" s="21">
         <v>51</v>
       </c>
-      <c r="BH6" s="35">
+      <c r="BH6" s="21">
         <v>52</v>
       </c>
-      <c r="BI6" s="36">
+      <c r="BI6" s="22">
         <v>53</v>
       </c>
-      <c r="BJ6" s="36">
+      <c r="BJ6" s="22">
         <v>54</v>
       </c>
-      <c r="BK6" s="36">
+      <c r="BK6" s="22">
         <v>55</v>
       </c>
-      <c r="BL6" s="36">
+      <c r="BL6" s="22">
         <v>56</v>
       </c>
-      <c r="BM6" s="35">
+      <c r="BM6" s="21">
         <v>57</v>
       </c>
-      <c r="BN6" s="35">
+      <c r="BN6" s="21">
         <v>58</v>
       </c>
-      <c r="BO6" s="35">
+      <c r="BO6" s="21">
         <v>59</v>
       </c>
-      <c r="BP6" s="35">
+      <c r="BP6" s="21">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="67"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1814,14 +1814,14 @@
       <c r="H7" s="5">
         <v>0</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1833,14 +1833,14 @@
       <c r="H8" s="5">
         <v>0</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="67"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1852,31 +1852,35 @@
       <c r="H9" s="5">
         <v>0</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="73">
+      <c r="B10" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="29">
         <v>1</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="29">
         <v>4</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74">
-        <v>0</v>
-      </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
+      <c r="F10" s="29">
+        <v>1</v>
+      </c>
+      <c r="G10" s="29">
+        <v>4</v>
+      </c>
+      <c r="H10" s="30">
+        <v>1</v>
+      </c>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="4">
@@ -1885,17 +1889,21 @@
       <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
       <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="C12" s="30" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="4">
@@ -1904,17 +1912,21 @@
       <c r="E12" s="4">
         <v>4</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4</v>
+      </c>
       <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31"/>
-      <c r="C13" s="30" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="4">
@@ -1923,16 +1935,20 @@
       <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4">
+        <v>3</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2</v>
+      </c>
       <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
     </row>
     <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1942,37 +1958,45 @@
       <c r="E14" s="4">
         <v>2</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
       <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="73">
+      <c r="B15" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="29">
         <v>5</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="29">
         <v>16</v>
       </c>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="74">
-        <v>0</v>
-      </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="F15" s="29">
+        <v>5</v>
+      </c>
+      <c r="G15" s="29">
+        <v>1</v>
+      </c>
+      <c r="H15" s="30">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31"/>
-      <c r="C16" s="30" t="s">
-        <v>26</v>
+      <c r="B16" s="18"/>
+      <c r="C16" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
@@ -1985,13 +2009,13 @@
       <c r="H16" s="5">
         <v>0</v>
       </c>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31"/>
-      <c r="C17" s="30" t="s">
-        <v>27</v>
+      <c r="B17" s="18"/>
+      <c r="C17" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="4">
         <v>7</v>
@@ -2004,13 +2028,13 @@
       <c r="H17" s="5">
         <v>0</v>
       </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31"/>
-      <c r="C18" s="30" t="s">
-        <v>28</v>
+      <c r="B18" s="18"/>
+      <c r="C18" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D18" s="4">
         <v>12</v>
@@ -2023,13 +2047,13 @@
       <c r="H18" s="5">
         <v>0</v>
       </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
     </row>
     <row r="19" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="31"/>
-      <c r="C19" s="30" t="s">
-        <v>29</v>
+      <c r="B19" s="18"/>
+      <c r="C19" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="D19" s="4">
         <v>14</v>
@@ -2042,13 +2066,13 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31"/>
-      <c r="C20" s="30" t="s">
-        <v>30</v>
+      <c r="B20" s="18"/>
+      <c r="C20" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D20" s="4">
         <v>15</v>
@@ -2061,13 +2085,13 @@
       <c r="H20" s="5">
         <v>0</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
     </row>
     <row r="21" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31"/>
-      <c r="C21" s="30" t="s">
-        <v>31</v>
+      <c r="B21" s="18"/>
+      <c r="C21" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="D21" s="4">
         <v>17</v>
@@ -2080,13 +2104,13 @@
       <c r="H21" s="5">
         <v>0</v>
       </c>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
     </row>
     <row r="22" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31"/>
-      <c r="C22" s="30" t="s">
-        <v>32</v>
+      <c r="B22" s="18"/>
+      <c r="C22" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="D22" s="4">
         <v>20</v>
@@ -2099,32 +2123,32 @@
       <c r="H22" s="5">
         <v>0</v>
       </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="73">
+      <c r="C23" s="61"/>
+      <c r="D23" s="29">
         <v>21</v>
       </c>
-      <c r="E23" s="73">
+      <c r="E23" s="29">
         <v>12</v>
       </c>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74">
-        <v>0</v>
-      </c>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="30">
+        <v>0</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
     </row>
     <row r="24" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="34"/>
-      <c r="C24" s="30" t="s">
-        <v>26</v>
+      <c r="B24" s="20"/>
+      <c r="C24" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="D24" s="4">
         <v>21</v>
@@ -2137,13 +2161,13 @@
       <c r="H24" s="5">
         <v>0</v>
       </c>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="34"/>
-      <c r="C25" s="30" t="s">
-        <v>27</v>
+      <c r="B25" s="20"/>
+      <c r="C25" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="D25" s="4">
         <v>22</v>
@@ -2156,13 +2180,13 @@
       <c r="H25" s="5">
         <v>0</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
     </row>
     <row r="26" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34"/>
-      <c r="C26" s="30" t="s">
-        <v>28</v>
+      <c r="B26" s="20"/>
+      <c r="C26" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D26" s="4">
         <v>24</v>
@@ -2175,13 +2199,13 @@
       <c r="H26" s="5">
         <v>0</v>
       </c>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="34"/>
-      <c r="C27" s="30" t="s">
-        <v>29</v>
+      <c r="B27" s="20"/>
+      <c r="C27" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="D27" s="4">
         <v>26</v>
@@ -2194,13 +2218,13 @@
       <c r="H27" s="5">
         <v>0</v>
       </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="34"/>
-      <c r="C28" s="30" t="s">
-        <v>30</v>
+      <c r="B28" s="20"/>
+      <c r="C28" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D28" s="4">
         <v>27</v>
@@ -2213,13 +2237,13 @@
       <c r="H28" s="5">
         <v>0</v>
       </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34"/>
-      <c r="C29" s="30" t="s">
-        <v>31</v>
+      <c r="B29" s="20"/>
+      <c r="C29" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="4">
         <v>28</v>
@@ -2232,13 +2256,13 @@
       <c r="H29" s="5">
         <v>0</v>
       </c>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="34"/>
-      <c r="C30" s="30" t="s">
-        <v>33</v>
+      <c r="B30" s="20"/>
+      <c r="C30" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="D30" s="4">
         <v>30</v>
@@ -2251,32 +2275,32 @@
       <c r="H30" s="5">
         <v>0</v>
       </c>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="73">
+      <c r="B31" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="61"/>
+      <c r="D31" s="29">
         <v>33</v>
       </c>
-      <c r="E31" s="73">
+      <c r="E31" s="29">
         <v>8</v>
       </c>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="74">
-        <v>0</v>
-      </c>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30">
+        <v>0</v>
+      </c>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34"/>
-      <c r="C32" s="30" t="s">
-        <v>34</v>
+      <c r="B32" s="20"/>
+      <c r="C32" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D32" s="4">
         <v>33</v>
@@ -2289,13 +2313,13 @@
       <c r="H32" s="5">
         <v>0</v>
       </c>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" spans="2:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="34"/>
-      <c r="C33" s="30" t="s">
-        <v>36</v>
+      <c r="B33" s="20"/>
+      <c r="C33" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="D33" s="4">
         <v>35</v>
@@ -2308,13 +2332,13 @@
       <c r="H33" s="5">
         <v>0</v>
       </c>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="30" t="s">
-        <v>38</v>
+      <c r="B34" s="20"/>
+      <c r="C34" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="D34" s="4">
         <v>37</v>
@@ -2327,32 +2351,32 @@
       <c r="H34" s="5">
         <v>0</v>
       </c>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="73">
+      <c r="B35" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="73">
+      <c r="C35" s="57"/>
+      <c r="D35" s="29">
+        <v>41</v>
+      </c>
+      <c r="E35" s="29">
         <v>8</v>
       </c>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="74">
-        <v>0</v>
-      </c>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="30">
+        <v>0</v>
+      </c>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
     </row>
     <row r="36" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="66"/>
-      <c r="C36" s="33" t="s">
-        <v>39</v>
+      <c r="B36" s="26"/>
+      <c r="C36" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="D36" s="4">
         <v>41</v>
@@ -2365,13 +2389,13 @@
       <c r="H36" s="5">
         <v>0</v>
       </c>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="66"/>
-      <c r="C37" s="33" t="s">
-        <v>40</v>
+      <c r="B37" s="26"/>
+      <c r="C37" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="D37" s="4">
         <v>43</v>
@@ -2384,13 +2408,13 @@
       <c r="H37" s="5">
         <v>0</v>
       </c>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
     </row>
     <row r="38" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="72"/>
-      <c r="C38" s="33" t="s">
-        <v>41</v>
+      <c r="B38" s="28"/>
+      <c r="C38" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="D38" s="4">
         <v>47</v>
@@ -2403,11 +2427,45 @@
       <c r="H38" s="5">
         <v>0</v>
       </c>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2424,40 +2482,6 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP38">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Added BackgroundsPanel and skeleton of associated avatars
</commit_message>
<xml_diff>
--- a/documentation/Gantt Chart.xlsx
+++ b/documentation/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578358BC-F156-4AB3-A780-858E035EED23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6738748D-1E91-4CFD-A5C9-19444AFFBFE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="855" yWindow="9210" windowWidth="19200" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -795,6 +795,99 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -810,9 +903,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,101 +921,11 @@
     <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1339,7 +1339,7 @@
   <dimension ref="B1:BP38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="U8" sqref="U8:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1365,62 +1365,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="67" t="s">
+      <c r="L2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="67" t="s">
+      <c r="R2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="69"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="35"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="65" t="s">
+      <c r="W2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="71"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="37"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="72" t="s">
+      <c r="AB2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="74"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="40"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="65" t="s">
+      <c r="AJ2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
     </row>
     <row r="3" spans="2:68" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1451,23 +1451,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="62" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="50" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1483,140 +1483,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="58">
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="42">
         <v>44120</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43">
         <v>44127</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="54">
+      <c r="L5" s="44"/>
+      <c r="M5" s="45">
         <v>44134</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54">
+      <c r="N5" s="45"/>
+      <c r="O5" s="45">
         <v>44141</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54">
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45">
         <v>44148</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="55">
+      <c r="R5" s="45"/>
+      <c r="S5" s="51">
         <v>44155</v>
       </c>
-      <c r="T5" s="55"/>
-      <c r="U5" s="54">
+      <c r="T5" s="51"/>
+      <c r="U5" s="45">
         <v>44162</v>
       </c>
-      <c r="V5" s="56"/>
-      <c r="W5" s="51">
+      <c r="V5" s="52"/>
+      <c r="W5" s="53">
         <v>44169</v>
       </c>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="50">
+      <c r="X5" s="53"/>
+      <c r="Y5" s="54">
         <v>44176</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="51">
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="53">
         <v>44183</v>
       </c>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="50">
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="54">
         <v>44190</v>
       </c>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="53">
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="56">
         <v>44197</v>
       </c>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="48">
+      <c r="AF5" s="57"/>
+      <c r="AG5" s="58">
         <v>44204</v>
       </c>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="47">
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="57">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="47"/>
-      <c r="AK5" s="48">
+      <c r="AJ5" s="57"/>
+      <c r="AK5" s="58">
         <v>44218</v>
       </c>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="47">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="57">
         <v>44225</v>
       </c>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="49">
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="59">
         <v>44232</v>
       </c>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="44">
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="61">
         <v>44239</v>
       </c>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="43">
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="60">
         <v>44246</v>
       </c>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="44">
+      <c r="AT5" s="60"/>
+      <c r="AU5" s="61">
         <v>44253</v>
       </c>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="45">
+      <c r="AV5" s="61"/>
+      <c r="AW5" s="73">
         <v>44260</v>
       </c>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="39">
+      <c r="AX5" s="74"/>
+      <c r="AY5" s="69">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="39"/>
-      <c r="BA5" s="46">
+      <c r="AZ5" s="69"/>
+      <c r="BA5" s="74">
         <v>44274</v>
       </c>
-      <c r="BB5" s="46"/>
-      <c r="BC5" s="39">
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="69">
         <v>44281</v>
       </c>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="41">
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="71">
         <v>44288</v>
       </c>
-      <c r="BF5" s="31"/>
-      <c r="BG5" s="42">
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="72">
         <v>44295</v>
       </c>
-      <c r="BH5" s="42"/>
-      <c r="BI5" s="31">
+      <c r="BH5" s="72"/>
+      <c r="BI5" s="62">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="31"/>
-      <c r="BK5" s="42">
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="72">
         <v>44309</v>
       </c>
-      <c r="BL5" s="42"/>
-      <c r="BM5" s="31">
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="62">
         <v>44316</v>
       </c>
-      <c r="BN5" s="32"/>
+      <c r="BN5" s="63"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1799,17 +1799,19 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
       <c r="E7" s="4">
         <v>4</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4">
+        <v>10</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="5">
         <v>0</v>
@@ -1818,10 +1820,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1837,10 +1839,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1856,10 +1858,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1971,10 +1973,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="61"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -2004,10 +2006,14 @@
       <c r="E16" s="4">
         <v>2</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="4">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3</v>
+      </c>
       <c r="H16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
@@ -2023,8 +2029,12 @@
       <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="F17" s="4">
+        <v>11</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
       <c r="H17" s="5">
         <v>0</v>
       </c>
@@ -2127,10 +2137,10 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="29">
         <v>21</v>
       </c>
@@ -2279,10 +2289,10 @@
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="61"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="29">
         <v>33</v>
       </c>
@@ -2355,10 +2365,10 @@
       <c r="J34" s="23"/>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="57" t="s">
+      <c r="B35" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="57"/>
+      <c r="C35" s="41"/>
       <c r="D35" s="29">
         <v>41</v>
       </c>
@@ -2432,40 +2442,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2482,6 +2458,40 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP38">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Removed node_modules from git repo
</commit_message>
<xml_diff>
--- a/documentation/Gantt Chart.xlsx
+++ b/documentation/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D328AF-2464-4506-85E1-6D7F340830C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361BCB86-35E3-4E4F-8AE5-D8AB1764E5AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,6 +795,108 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -824,108 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1339,7 +1339,7 @@
   <dimension ref="B1:BP38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BA28" sqref="BA28"/>
+      <selection activeCell="BG12" sqref="BG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1365,62 +1365,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="66"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="69"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="35"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="69"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="37"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="71"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="38" t="s">
+      <c r="AB2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="40"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="74"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="31" t="s">
+      <c r="AJ2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
+      <c r="AK2" s="66"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
     </row>
     <row r="3" spans="2:68" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1451,23 +1451,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="48" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="64" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1483,140 +1483,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="42">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="58">
         <v>44120</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43">
+      <c r="J5" s="59"/>
+      <c r="K5" s="59">
         <v>44127</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45">
+      <c r="L5" s="60"/>
+      <c r="M5" s="54">
         <v>44134</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45">
+      <c r="N5" s="54"/>
+      <c r="O5" s="54">
         <v>44141</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45">
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54">
         <v>44148</v>
       </c>
-      <c r="R5" s="45"/>
-      <c r="S5" s="51">
+      <c r="R5" s="54"/>
+      <c r="S5" s="55">
         <v>44155</v>
       </c>
-      <c r="T5" s="51"/>
-      <c r="U5" s="45">
+      <c r="T5" s="55"/>
+      <c r="U5" s="54">
         <v>44162</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53">
+      <c r="V5" s="56"/>
+      <c r="W5" s="51">
         <v>44169</v>
       </c>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="54">
+      <c r="X5" s="51"/>
+      <c r="Y5" s="50">
         <v>44176</v>
       </c>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="53">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="51">
         <v>44183</v>
       </c>
-      <c r="AB5" s="53"/>
-      <c r="AC5" s="54">
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="50">
         <v>44190</v>
       </c>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="56">
+      <c r="AD5" s="52"/>
+      <c r="AE5" s="53">
         <v>44197</v>
       </c>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="58">
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="48">
         <v>44204</v>
       </c>
-      <c r="AH5" s="58"/>
-      <c r="AI5" s="57">
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="47">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="58">
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="48">
         <v>44218</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="57">
+      <c r="AL5" s="48"/>
+      <c r="AM5" s="47">
         <v>44225</v>
       </c>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="59">
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="49">
         <v>44232</v>
       </c>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="61">
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="44">
         <v>44239</v>
       </c>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="60">
+      <c r="AR5" s="44"/>
+      <c r="AS5" s="43">
         <v>44246</v>
       </c>
-      <c r="AT5" s="60"/>
-      <c r="AU5" s="61">
+      <c r="AT5" s="43"/>
+      <c r="AU5" s="44">
         <v>44253</v>
       </c>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="73">
+      <c r="AV5" s="44"/>
+      <c r="AW5" s="45">
         <v>44260</v>
       </c>
-      <c r="AX5" s="74"/>
-      <c r="AY5" s="69">
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="39">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="74">
+      <c r="AZ5" s="39"/>
+      <c r="BA5" s="46">
         <v>44274</v>
       </c>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="69">
+      <c r="BB5" s="46"/>
+      <c r="BC5" s="39">
         <v>44281</v>
       </c>
-      <c r="BD5" s="70"/>
-      <c r="BE5" s="71">
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="41">
         <v>44288</v>
       </c>
-      <c r="BF5" s="62"/>
-      <c r="BG5" s="72">
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="42">
         <v>44295</v>
       </c>
-      <c r="BH5" s="72"/>
-      <c r="BI5" s="62">
+      <c r="BH5" s="42"/>
+      <c r="BI5" s="31">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="62"/>
-      <c r="BK5" s="72">
+      <c r="BJ5" s="31"/>
+      <c r="BK5" s="42">
         <v>44309</v>
       </c>
-      <c r="BL5" s="72"/>
-      <c r="BM5" s="62">
+      <c r="BL5" s="42"/>
+      <c r="BM5" s="31">
         <v>44316</v>
       </c>
-      <c r="BN5" s="63"/>
+      <c r="BN5" s="32"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1799,10 +1799,10 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1822,10 +1822,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1841,10 +1841,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1860,10 +1860,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1975,10 +1975,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -2143,10 +2143,10 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="47"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="29">
         <v>21</v>
       </c>
@@ -2295,10 +2295,10 @@
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="29">
         <v>33</v>
       </c>
@@ -2371,10 +2371,10 @@
       <c r="J34" s="23"/>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="29">
         <v>41</v>
       </c>
@@ -2448,6 +2448,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2464,40 +2498,6 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP38">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Added SkillsPanel, with tables for displaying skills
</commit_message>
<xml_diff>
--- a/documentation/Gantt Chart.xlsx
+++ b/documentation/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D328AF-2464-4506-85E1-6D7F340830C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC330A25-841D-4EC9-8499-88EE00F93BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,6 +795,108 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -824,108 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1339,7 +1339,7 @@
   <dimension ref="B1:BP38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BA28" sqref="BA28"/>
+      <selection activeCell="AP15" sqref="AP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1365,62 +1365,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="66"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="69"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="35"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="69"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="37"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="71"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="38" t="s">
+      <c r="AB2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="40"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="74"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="31" t="s">
+      <c r="AJ2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
+      <c r="AK2" s="66"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
     </row>
     <row r="3" spans="2:68" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1451,23 +1451,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="64" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1483,140 +1483,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="42">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="58">
         <v>44120</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43">
+      <c r="J5" s="59"/>
+      <c r="K5" s="59">
         <v>44127</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45">
+      <c r="L5" s="60"/>
+      <c r="M5" s="54">
         <v>44134</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45">
+      <c r="N5" s="54"/>
+      <c r="O5" s="54">
         <v>44141</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45">
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54">
         <v>44148</v>
       </c>
-      <c r="R5" s="45"/>
-      <c r="S5" s="51">
+      <c r="R5" s="54"/>
+      <c r="S5" s="55">
         <v>44155</v>
       </c>
-      <c r="T5" s="51"/>
-      <c r="U5" s="45">
+      <c r="T5" s="55"/>
+      <c r="U5" s="54">
         <v>44162</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53">
+      <c r="V5" s="56"/>
+      <c r="W5" s="51">
         <v>44169</v>
       </c>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="54">
+      <c r="X5" s="51"/>
+      <c r="Y5" s="50">
         <v>44176</v>
       </c>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="53">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="51">
         <v>44183</v>
       </c>
-      <c r="AB5" s="53"/>
-      <c r="AC5" s="54">
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="50">
         <v>44190</v>
       </c>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="56">
+      <c r="AD5" s="52"/>
+      <c r="AE5" s="53">
         <v>44197</v>
       </c>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="58">
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="48">
         <v>44204</v>
       </c>
-      <c r="AH5" s="58"/>
-      <c r="AI5" s="57">
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="47">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="58">
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="48">
         <v>44218</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="57">
+      <c r="AL5" s="48"/>
+      <c r="AM5" s="47">
         <v>44225</v>
       </c>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="59">
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="49">
         <v>44232</v>
       </c>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="61">
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="44">
         <v>44239</v>
       </c>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="60">
+      <c r="AR5" s="44"/>
+      <c r="AS5" s="43">
         <v>44246</v>
       </c>
-      <c r="AT5" s="60"/>
-      <c r="AU5" s="61">
+      <c r="AT5" s="43"/>
+      <c r="AU5" s="44">
         <v>44253</v>
       </c>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="73">
+      <c r="AV5" s="44"/>
+      <c r="AW5" s="45">
         <v>44260</v>
       </c>
-      <c r="AX5" s="74"/>
-      <c r="AY5" s="69">
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="39">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="74">
+      <c r="AZ5" s="39"/>
+      <c r="BA5" s="46">
         <v>44274</v>
       </c>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="69">
+      <c r="BB5" s="46"/>
+      <c r="BC5" s="39">
         <v>44281</v>
       </c>
-      <c r="BD5" s="70"/>
-      <c r="BE5" s="71">
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="41">
         <v>44288</v>
       </c>
-      <c r="BF5" s="62"/>
-      <c r="BG5" s="72">
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="42">
         <v>44295</v>
       </c>
-      <c r="BH5" s="72"/>
-      <c r="BI5" s="62">
+      <c r="BH5" s="42"/>
+      <c r="BI5" s="31">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="62"/>
-      <c r="BK5" s="72">
+      <c r="BJ5" s="31"/>
+      <c r="BK5" s="42">
         <v>44309</v>
       </c>
-      <c r="BL5" s="72"/>
-      <c r="BM5" s="62">
+      <c r="BL5" s="42"/>
+      <c r="BM5" s="31">
         <v>44316</v>
       </c>
-      <c r="BN5" s="63"/>
+      <c r="BN5" s="32"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1799,10 +1799,10 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1822,10 +1822,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1841,10 +1841,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1860,10 +1860,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1975,10 +1975,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="30">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
@@ -2058,10 +2058,10 @@
         <v>12</v>
       </c>
       <c r="G18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
@@ -2077,8 +2077,12 @@
       <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="F19" s="4">
+        <v>14</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
       <c r="H19" s="5">
         <v>0</v>
       </c>
@@ -2143,10 +2147,10 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="47"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="29">
         <v>21</v>
       </c>
@@ -2295,10 +2299,10 @@
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="29">
         <v>33</v>
       </c>
@@ -2371,10 +2375,10 @@
       <c r="J34" s="23"/>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="29">
         <v>41</v>
       </c>
@@ -2448,6 +2452,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2464,40 +2502,6 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP38">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>